<commit_message>
View Profile Info Done
</commit_message>
<xml_diff>
--- a/KTLT-19CLC1-2-FinalProjectPlan.xlsx
+++ b/KTLT-19CLC1-2-FinalProjectPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="140">
   <si>
     <t>Project Planner</t>
   </si>
@@ -615,6 +615,9 @@
   </si>
   <si>
     <t>+84355509301</t>
+  </si>
+  <si>
+    <t>Kha, Hoang</t>
   </si>
 </sst>
 </file>
@@ -1926,7 +1929,7 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -2143,12 +2146,12 @@
   </sheetPr>
   <dimension ref="A1:BO81"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="K13" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="10" ySplit="6" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2727,7 +2730,7 @@
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="29" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="E9" s="14">
         <v>2</v>
@@ -2750,7 +2753,7 @@
       </c>
       <c r="C10" s="28"/>
       <c r="D10" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E10" s="14">
         <v>2</v>

</xml_diff>

<commit_message>
Manually add new student to class done
update report progression too
</commit_message>
<xml_diff>
--- a/KTLT-19CLC1-2-FinalProjectPlan.xlsx
+++ b/KTLT-19CLC1-2-FinalProjectPlan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7713A9B-9CD7-457B-ABFD-C1DDBAA6D532}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3793C460-B993-4CCC-AC30-4AF6B8D1F038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="4110" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -2144,7 +2144,7 @@
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2902,9 +2902,15 @@
       <c r="F16" s="14">
         <v>4</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="15"/>
+      <c r="G16" s="14">
+        <v>7</v>
+      </c>
+      <c r="H16" s="14">
+        <v>1</v>
+      </c>
+      <c r="I16" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="47">

</xml_diff>

<commit_message>
View students of a class
</commit_message>
<xml_diff>
--- a/KTLT-19CLC1-2-FinalProjectPlan.xlsx
+++ b/KTLT-19CLC1-2-FinalProjectPlan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CFD380-29C8-4B19-8EFF-0DADDB72F500}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926DAC91-B1CB-4ADC-9652-F2951623E3B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -2140,11 +2140,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="K16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="K13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2977,9 +2977,15 @@
       <c r="F19" s="14">
         <v>4</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="15"/>
+      <c r="G19" s="14">
+        <v>7</v>
+      </c>
+      <c r="H19" s="14">
+        <v>1</v>
+      </c>
+      <c r="I19" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="47">
@@ -2998,9 +3004,15 @@
       <c r="F20" s="14">
         <v>4</v>
       </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="15"/>
+      <c r="G20" s="14">
+        <v>7</v>
+      </c>
+      <c r="H20" s="14">
+        <v>1</v>
+      </c>
+      <c r="I20" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="47">
@@ -3019,9 +3031,15 @@
       <c r="F21" s="14">
         <v>4</v>
       </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="15"/>
+      <c r="G21" s="14">
+        <v>7</v>
+      </c>
+      <c r="H21" s="14">
+        <v>1</v>
+      </c>
+      <c r="I21" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="46">

</xml_diff>

<commit_message>
Gom code lại + update report
</commit_message>
<xml_diff>
--- a/KTLT-19CLC1-2-FinalProjectPlan.xlsx
+++ b/KTLT-19CLC1-2-FinalProjectPlan.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBA5A94-67B2-469F-899C-D1D322DD41EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B163E9-3CF7-4353-989C-6B719FC6B540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="141">
   <si>
     <t>Project Planner</t>
   </si>
@@ -611,6 +611,9 @@
   </si>
   <si>
     <t>Kha, Hoang</t>
+  </si>
+  <si>
+    <t>Hoang, Phuoc</t>
   </si>
 </sst>
 </file>
@@ -2140,11 +2143,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="K19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="K16" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="K27" sqref="K27"/>
+      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3064,7 +3067,7 @@
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="29" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E23" s="14">
         <v>10</v>
@@ -3072,7 +3075,9 @@
       <c r="F23" s="14">
         <v>3</v>
       </c>
-      <c r="G23" s="14"/>
+      <c r="G23" s="14">
+        <v>12</v>
+      </c>
       <c r="H23" s="14"/>
       <c r="I23" s="15"/>
     </row>
@@ -3093,7 +3098,9 @@
       <c r="F24" s="14">
         <v>3</v>
       </c>
-      <c r="G24" s="14"/>
+      <c r="G24" s="14">
+        <v>14</v>
+      </c>
       <c r="H24" s="14"/>
       <c r="I24" s="15"/>
     </row>
@@ -3106,7 +3113,7 @@
       </c>
       <c r="C25" s="28"/>
       <c r="D25" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E25" s="14">
         <v>10</v>
@@ -3114,7 +3121,9 @@
       <c r="F25" s="14">
         <v>3</v>
       </c>
-      <c r="G25" s="14"/>
+      <c r="G25" s="14">
+        <v>14</v>
+      </c>
       <c r="H25" s="14"/>
       <c r="I25" s="15"/>
     </row>
@@ -3135,7 +3144,9 @@
       <c r="F26" s="14">
         <v>3</v>
       </c>
-      <c r="G26" s="14"/>
+      <c r="G26" s="14">
+        <v>14</v>
+      </c>
       <c r="H26" s="14"/>
       <c r="I26" s="15"/>
     </row>
@@ -3156,7 +3167,9 @@
       <c r="F27" s="14">
         <v>3</v>
       </c>
-      <c r="G27" s="14"/>
+      <c r="G27" s="14">
+        <v>14</v>
+      </c>
       <c r="H27" s="14"/>
       <c r="I27" s="15"/>
     </row>
@@ -3177,7 +3190,9 @@
       <c r="F28" s="14">
         <v>3</v>
       </c>
-      <c r="G28" s="14"/>
+      <c r="G28" s="14">
+        <v>14</v>
+      </c>
       <c r="H28" s="14"/>
       <c r="I28" s="15"/>
     </row>
@@ -3198,7 +3213,9 @@
       <c r="F29" s="14">
         <v>3</v>
       </c>
-      <c r="G29" s="14"/>
+      <c r="G29" s="14">
+        <v>14</v>
+      </c>
       <c r="H29" s="14"/>
       <c r="I29" s="15"/>
     </row>
@@ -3219,7 +3236,9 @@
       <c r="F30" s="14">
         <v>3</v>
       </c>
-      <c r="G30" s="14"/>
+      <c r="G30" s="14">
+        <v>14</v>
+      </c>
       <c r="H30" s="14"/>
       <c r="I30" s="15"/>
     </row>
@@ -3240,7 +3259,9 @@
       <c r="F31" s="14">
         <v>3</v>
       </c>
-      <c r="G31" s="14"/>
+      <c r="G31" s="14">
+        <v>14</v>
+      </c>
       <c r="H31" s="14"/>
       <c r="I31" s="15"/>
     </row>
@@ -3261,7 +3282,9 @@
       <c r="F32" s="14">
         <v>3</v>
       </c>
-      <c r="G32" s="14"/>
+      <c r="G32" s="14">
+        <v>14</v>
+      </c>
       <c r="H32" s="14"/>
       <c r="I32" s="15"/>
     </row>
@@ -3282,7 +3305,9 @@
       <c r="F33" s="14">
         <v>3</v>
       </c>
-      <c r="G33" s="14"/>
+      <c r="G33" s="14">
+        <v>14</v>
+      </c>
       <c r="H33" s="14"/>
       <c r="I33" s="15"/>
     </row>

</xml_diff>

<commit_message>
Remove hoàn chỉnh nha ae
remove hoàn chỉnh
</commit_message>
<xml_diff>
--- a/KTLT-19CLC1-2-FinalProjectPlan.xlsx
+++ b/KTLT-19CLC1-2-FinalProjectPlan.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1327BB-8120-41B2-AB33-372113F8611A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -619,7 +618,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="d/m"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -1284,15 +1283,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Activity" xfId="2"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
-    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Label" xfId="5"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Percent Complete" xfId="6"/>
+    <cellStyle name="Period Headers" xfId="3"/>
+    <cellStyle name="Period Highlight Control" xfId="7"/>
+    <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -1522,13 +1521,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="C6:F11" totalsRowShown="0">
-  <autoFilter ref="C6:F11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C6:F11" totalsRowShown="0">
+  <autoFilter ref="C6:F11"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Email"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Slack username" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Phone"/>
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="3" name="Email"/>
+    <tableColumn id="4" name="Slack username" dataDxfId="10"/>
+    <tableColumn id="2" name="Phone"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1760,7 +1759,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
@@ -1919,7 +1918,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
@@ -2119,9 +2118,9 @@
     <mergeCell ref="A1:G3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D7" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="D9" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="D8" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D7" r:id="rId1"/>
+    <hyperlink ref="D9" r:id="rId2"/>
+    <hyperlink ref="D8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -2135,7 +2134,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
@@ -2143,11 +2142,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="K13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="K14" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2951,7 +2950,7 @@
       </c>
       <c r="C18" s="28"/>
       <c r="D18" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E18" s="14">
         <v>5</v>
@@ -3704,7 +3703,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="-0.499984740745262"/>
   </sheetPr>

</xml_diff>

<commit_message>
FIX BUG + Update Code Flexibility
Xong phần Remove Course + Remove student from Course + View All Student from class + course
</commit_message>
<xml_diff>
--- a/KTLT-19CLC1-2-FinalProjectPlan.xlsx
+++ b/KTLT-19CLC1-2-FinalProjectPlan.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7DACAC-5AA6-41F3-AC2F-FC546B79E970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -618,7 +619,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="d/m"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -1283,15 +1284,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Activity" xfId="2"/>
+    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
-    <cellStyle name="Label" xfId="5"/>
+    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6"/>
-    <cellStyle name="Period Headers" xfId="3"/>
-    <cellStyle name="Period Highlight Control" xfId="7"/>
-    <cellStyle name="Project Headers" xfId="4"/>
+    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -1521,13 +1522,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C6:F11" totalsRowShown="0">
-  <autoFilter ref="C6:F11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="C6:F11" totalsRowShown="0">
+  <autoFilter ref="C6:F11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="3" name="Email"/>
-    <tableColumn id="4" name="Slack username" dataDxfId="10"/>
-    <tableColumn id="2" name="Phone"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Email"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Slack username" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Phone"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1759,7 +1760,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
@@ -1918,7 +1919,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
@@ -2118,9 +2119,9 @@
     <mergeCell ref="A1:G3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D7" r:id="rId1"/>
-    <hyperlink ref="D9" r:id="rId2"/>
-    <hyperlink ref="D8" r:id="rId3"/>
+    <hyperlink ref="D7" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D9" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -2134,7 +2135,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
@@ -2142,11 +2143,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="K14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="K22" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="I18" sqref="I18"/>
+      <selection pane="bottomRight" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3089,8 +3090,12 @@
       <c r="G23" s="14">
         <v>12</v>
       </c>
-      <c r="H23" s="14"/>
-      <c r="I23" s="15"/>
+      <c r="H23" s="14">
+        <v>5</v>
+      </c>
+      <c r="I23" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="47">
@@ -3112,8 +3117,12 @@
       <c r="G24" s="14">
         <v>14</v>
       </c>
-      <c r="H24" s="14"/>
-      <c r="I24" s="15"/>
+      <c r="H24" s="14">
+        <v>5</v>
+      </c>
+      <c r="I24" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47">
@@ -3181,8 +3190,12 @@
       <c r="G27" s="14">
         <v>14</v>
       </c>
-      <c r="H27" s="14"/>
-      <c r="I27" s="15"/>
+      <c r="H27" s="14">
+        <v>5</v>
+      </c>
+      <c r="I27" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="47">
@@ -3204,8 +3217,12 @@
       <c r="G28" s="14">
         <v>14</v>
       </c>
-      <c r="H28" s="14"/>
-      <c r="I28" s="15"/>
+      <c r="H28" s="14">
+        <v>6</v>
+      </c>
+      <c r="I28" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="47">
@@ -3273,8 +3290,12 @@
       <c r="G31" s="14">
         <v>14</v>
       </c>
-      <c r="H31" s="14"/>
-      <c r="I31" s="15"/>
+      <c r="H31" s="14">
+        <v>5</v>
+      </c>
+      <c r="I31" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="47">
@@ -3319,8 +3340,12 @@
       <c r="G33" s="14">
         <v>14</v>
       </c>
-      <c r="H33" s="14"/>
-      <c r="I33" s="15"/>
+      <c r="H33" s="14">
+        <v>5</v>
+      </c>
+      <c r="I33" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="46">
@@ -3709,7 +3734,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="-0.499984740745262"/>
   </sheetPr>

</xml_diff>

<commit_message>
Import_course + Academic của Hoàng Béo
update report + update bài dùm
</commit_message>
<xml_diff>
--- a/KTLT-19CLC1-2-FinalProjectPlan.xlsx
+++ b/KTLT-19CLC1-2-FinalProjectPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7DACAC-5AA6-41F3-AC2F-FC546B79E970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C997D70B-2927-4E66-9D40-98E34F72A5C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2143,11 +2143,11 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="K22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="K25" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="J30" sqref="J30"/>
+      <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
File Tạm Thời :))
</commit_message>
<xml_diff>
--- a/KTLT-19CLC1-2-FinalProjectPlan.xlsx
+++ b/KTLT-19CLC1-2-FinalProjectPlan.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8256ED-1EA0-4868-A523-A3E4782D86BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="144">
   <si>
     <t>Project Planner</t>
   </si>
@@ -577,15 +576,6 @@
     <t>phhoang</t>
   </si>
   <si>
-    <t>Minh Kha</t>
-  </si>
-  <si>
-    <t>Huy Hoàng</t>
-  </si>
-  <si>
-    <t>Thịnh Phước</t>
-  </si>
-  <si>
     <t>lhtphuoc</t>
   </si>
   <si>
@@ -604,9 +594,6 @@
     <t>Hoang</t>
   </si>
   <si>
-    <t>+84973597990</t>
-  </si>
-  <si>
     <t>+84355509301</t>
   </si>
   <si>
@@ -617,19 +604,37 @@
   </si>
   <si>
     <t>Hoang + Kha</t>
+  </si>
+  <si>
+    <t>Lê Hoàng Thịnh Phước</t>
+  </si>
+  <si>
+    <t>Phan Huy Hoàng</t>
+  </si>
+  <si>
+    <t>Team's Performance (by group leader)</t>
+  </si>
+  <si>
+    <t>Nguyễn Minh Kha</t>
+  </si>
+  <si>
+    <t>Phuoc + Hoang</t>
+  </si>
+  <si>
+    <t>84973597990</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="d/m"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="166" formatCode="dd/mmm/yy"/>
     <numFmt numFmtId="167" formatCode="dd\ mmm\ yy"/>
   </numFmts>
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -922,6 +927,13 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -972,7 +984,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1056,6 +1068,90 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -1084,7 +1180,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1169,9 +1265,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1279,6 +1372,36 @@
     <xf numFmtId="49" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1287,15 +1410,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Activity" xfId="2"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
-    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Label" xfId="5"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Percent Complete" xfId="6"/>
+    <cellStyle name="Period Headers" xfId="3"/>
+    <cellStyle name="Period Highlight Control" xfId="7"/>
+    <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -1525,13 +1648,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="C6:F11" totalsRowShown="0">
-  <autoFilter ref="C6:F11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C6:F11" totalsRowShown="0">
+  <autoFilter ref="C6:F11"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Email"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Slack username" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Phone"/>
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="3" name="Email"/>
+    <tableColumn id="4" name="Slack username" dataDxfId="10"/>
+    <tableColumn id="2" name="Phone"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1763,14 +1886,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,36 +1906,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
+      <c r="A3" s="79"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
     </row>
     <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
@@ -1911,6 +2034,115 @@
       <c r="C16" s="21" t="s">
         <v>44</v>
       </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="77" t="s">
+        <v>140</v>
+      </c>
+      <c r="B19" s="69"/>
+      <c r="C19" s="70"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="78" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" s="69"/>
+      <c r="C20" s="70"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="71"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="73"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="71"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="73"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="71"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="73"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="71"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="73"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="74"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="76"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="78" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="72"/>
+      <c r="C26" s="73"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="71"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="73"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="71"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="73"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="71"/>
+      <c r="B29" s="72"/>
+      <c r="C29" s="73"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="71"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="73"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="71"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="73"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="78" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="69"/>
+      <c r="C32" s="70"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="71"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="73"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="71"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="73"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="71"/>
+      <c r="B35" s="72"/>
+      <c r="C35" s="73"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="71"/>
+      <c r="B36" s="72"/>
+      <c r="C36" s="73"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="74"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="76"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="71"/>
+      <c r="B38" s="72"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1922,53 +2154,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.625" customWidth="1"/>
-    <col min="3" max="3" width="15.875" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
     <col min="5" max="5" width="16.875" customWidth="1"/>
     <col min="6" max="6" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
     </row>
     <row r="3" spans="1:7" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
+      <c r="A3" s="79"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
@@ -1999,43 +2231,43 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="17"/>
       <c r="C7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D7" s="40" t="s">
-        <v>132</v>
+        <v>141</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>129</v>
       </c>
       <c r="E7" t="s">
         <v>126</v>
       </c>
-      <c r="F7" s="68" t="s">
-        <v>137</v>
+      <c r="F7" s="67" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="17"/>
       <c r="C8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>134</v>
+        <v>139</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>131</v>
       </c>
       <c r="E8" t="s">
         <v>127</v>
       </c>
-      <c r="F8" s="69" t="s">
-        <v>138</v>
+      <c r="F8" s="68" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="17"/>
       <c r="C9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="D9" s="40" t="s">
-        <v>133</v>
-      </c>
       <c r="E9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F9">
         <v>84945093057</v>
@@ -2043,11 +2275,11 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
-      <c r="D10" s="40"/>
+      <c r="D10" s="39"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="17"/>
-      <c r="D11" s="40"/>
+      <c r="D11" s="39"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="17"/>
@@ -2062,7 +2294,7 @@
       <c r="E13" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="52">
+      <c r="F13" s="51">
         <v>43941</v>
       </c>
     </row>
@@ -2076,44 +2308,46 @@
       <c r="E14" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="32"/>
+      <c r="F14" s="51">
+        <v>44002</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="17"/>
       <c r="C15" s="30"/>
     </row>
     <row r="21" spans="3:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="C21" s="62" t="s">
+      <c r="C21" s="61" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="22" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C22" s="57" t="s">
+      <c r="C22" s="56" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="23" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="57" t="s">
+      <c r="C23" s="56" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="24" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C24" s="57" t="s">
+      <c r="C24" s="56" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="25" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C25" s="57" t="s">
+      <c r="C25" s="56" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="27" spans="3:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="C27" s="67" t="s">
+      <c r="C27" s="66" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="28" spans="3:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="66" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2122,14 +2356,14 @@
     <mergeCell ref="A1:G3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D7" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="D9" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="D8" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D7" r:id="rId1"/>
+    <hyperlink ref="D9" r:id="rId2"/>
+    <hyperlink ref="D8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
   <ignoredErrors>
-    <ignoredError sqref="F7:F8" numberStoredAsText="1"/>
+    <ignoredError sqref="F8" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId5"/>
@@ -2138,7 +2372,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
@@ -2146,16 +2380,16 @@
   <dimension ref="A1:BO81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="L37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="6" topLeftCell="K10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="H49" sqref="H49"/>
+      <selection pane="bottomRight" activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6" style="45" customWidth="1"/>
+    <col min="1" max="1" width="6" style="44" customWidth="1"/>
     <col min="2" max="2" width="36.875" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.125" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.125" style="2" customWidth="1"/>
@@ -2190,26 +2424,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:67" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
     </row>
     <row r="2" spans="1:67" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
       <c r="K2" s="7" t="s">
         <v>14</v>
       </c>
@@ -2247,14 +2481,14 @@
       </c>
     </row>
     <row r="3" spans="1:67" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
@@ -2265,189 +2499,189 @@
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="34" t="s">
         <v>7</v>
       </c>
       <c r="J4" s="4"/>
-      <c r="K4" s="56">
+      <c r="K4" s="55">
         <v>43927</v>
       </c>
-      <c r="L4" s="37"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="R4" s="56">
+      <c r="L4" s="36"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="R4" s="55">
         <v>43934</v>
       </c>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="38"/>
-      <c r="V4" s="38"/>
-      <c r="W4" s="53"/>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="56">
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="52"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="55">
         <v>43941</v>
       </c>
-      <c r="Z4" s="37"/>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="38"/>
-      <c r="AC4" s="38"/>
-      <c r="AD4" s="38"/>
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="37"/>
+      <c r="AC4" s="37"/>
+      <c r="AD4" s="37"/>
       <c r="AE4" s="1"/>
-      <c r="AF4" s="56">
+      <c r="AF4" s="55">
         <v>43948</v>
       </c>
-      <c r="AG4" s="38"/>
-      <c r="AH4" s="38"/>
-      <c r="AI4" s="38"/>
-      <c r="AJ4" s="38"/>
-      <c r="AK4" s="53"/>
-      <c r="AL4" s="38"/>
-      <c r="AM4" s="56">
+      <c r="AG4" s="37"/>
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="37"/>
+      <c r="AJ4" s="37"/>
+      <c r="AK4" s="52"/>
+      <c r="AL4" s="37"/>
+      <c r="AM4" s="55">
         <v>43955</v>
       </c>
-      <c r="AN4" s="37"/>
-      <c r="AO4" s="38"/>
-      <c r="AP4" s="38"/>
-      <c r="AQ4" s="38"/>
-      <c r="AR4" s="38"/>
+      <c r="AN4" s="36"/>
+      <c r="AO4" s="37"/>
+      <c r="AP4" s="37"/>
+      <c r="AQ4" s="37"/>
+      <c r="AR4" s="37"/>
       <c r="AS4" s="1"/>
-      <c r="AT4" s="56">
+      <c r="AT4" s="55">
         <v>43962</v>
       </c>
-      <c r="AU4" s="38"/>
-      <c r="AV4" s="38"/>
-      <c r="AW4" s="38"/>
-      <c r="AX4" s="38"/>
-      <c r="AY4" s="53"/>
-      <c r="AZ4" s="38"/>
-      <c r="BA4" s="56">
+      <c r="AU4" s="37"/>
+      <c r="AV4" s="37"/>
+      <c r="AW4" s="37"/>
+      <c r="AX4" s="37"/>
+      <c r="AY4" s="52"/>
+      <c r="AZ4" s="37"/>
+      <c r="BA4" s="55">
         <v>43969</v>
       </c>
-      <c r="BB4" s="37"/>
-      <c r="BC4" s="38"/>
-      <c r="BD4" s="38"/>
-      <c r="BE4" s="38"/>
-      <c r="BF4" s="38"/>
+      <c r="BB4" s="36"/>
+      <c r="BC4" s="37"/>
+      <c r="BD4" s="37"/>
+      <c r="BE4" s="37"/>
+      <c r="BF4" s="37"/>
       <c r="BG4" s="1"/>
-      <c r="BH4" s="56">
+      <c r="BH4" s="55">
         <v>43976</v>
       </c>
-      <c r="BI4" s="38"/>
-      <c r="BJ4" s="38"/>
-      <c r="BK4" s="38"/>
-      <c r="BL4" s="38"/>
-      <c r="BM4" s="53"/>
-      <c r="BN4" s="38"/>
-      <c r="BO4" s="56">
+      <c r="BI4" s="37"/>
+      <c r="BJ4" s="37"/>
+      <c r="BK4" s="37"/>
+      <c r="BL4" s="37"/>
+      <c r="BM4" s="52"/>
+      <c r="BN4" s="37"/>
+      <c r="BO4" s="55">
         <v>43983</v>
       </c>
     </row>
     <row r="5" spans="1:67" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="34" t="s">
         <v>8</v>
       </c>
       <c r="J5" s="4"/>
-      <c r="K5" s="36" t="s">
+      <c r="K5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="37"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
-      <c r="W5" s="38"/>
-      <c r="X5" s="38"/>
-      <c r="Y5" s="38"/>
-      <c r="Z5" s="38"/>
-      <c r="AA5" s="38"/>
-      <c r="AB5" s="38"/>
-      <c r="AC5" s="38"/>
-      <c r="AD5" s="38"/>
-      <c r="AE5" s="39"/>
-      <c r="AF5" s="38"/>
-      <c r="AG5" s="39"/>
-      <c r="AH5" s="39"/>
-      <c r="AI5" s="39"/>
-      <c r="AJ5" s="39"/>
-      <c r="AK5" s="39"/>
-      <c r="AL5" s="38"/>
-      <c r="AM5" s="39"/>
-      <c r="AN5" s="39"/>
-      <c r="AO5" s="39"/>
-      <c r="AP5" s="39"/>
-      <c r="AQ5" s="39"/>
-      <c r="AR5" s="39"/>
-      <c r="AS5" s="39"/>
-      <c r="AT5" s="39"/>
-      <c r="AU5" s="39"/>
-      <c r="AV5" s="39"/>
-      <c r="AW5" s="39"/>
-      <c r="AX5" s="39"/>
-      <c r="AY5" s="39"/>
-      <c r="AZ5" s="38"/>
-      <c r="BA5" s="39"/>
-      <c r="BB5" s="39"/>
-      <c r="BC5" s="39"/>
-      <c r="BD5" s="39"/>
-      <c r="BE5" s="39"/>
-      <c r="BF5" s="38"/>
-      <c r="BG5" s="39"/>
-      <c r="BH5" s="39"/>
-      <c r="BI5" s="39"/>
-      <c r="BJ5" s="39"/>
-      <c r="BK5" s="39"/>
-      <c r="BL5" s="39"/>
-      <c r="BM5" s="39"/>
-      <c r="BN5" s="38"/>
-      <c r="BO5" s="39"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37"/>
+      <c r="X5" s="37"/>
+      <c r="Y5" s="37"/>
+      <c r="Z5" s="37"/>
+      <c r="AA5" s="37"/>
+      <c r="AB5" s="37"/>
+      <c r="AC5" s="37"/>
+      <c r="AD5" s="37"/>
+      <c r="AE5" s="38"/>
+      <c r="AF5" s="37"/>
+      <c r="AG5" s="38"/>
+      <c r="AH5" s="38"/>
+      <c r="AI5" s="38"/>
+      <c r="AJ5" s="38"/>
+      <c r="AK5" s="38"/>
+      <c r="AL5" s="37"/>
+      <c r="AM5" s="38"/>
+      <c r="AN5" s="38"/>
+      <c r="AO5" s="38"/>
+      <c r="AP5" s="38"/>
+      <c r="AQ5" s="38"/>
+      <c r="AR5" s="38"/>
+      <c r="AS5" s="38"/>
+      <c r="AT5" s="38"/>
+      <c r="AU5" s="38"/>
+      <c r="AV5" s="38"/>
+      <c r="AW5" s="38"/>
+      <c r="AX5" s="38"/>
+      <c r="AY5" s="38"/>
+      <c r="AZ5" s="37"/>
+      <c r="BA5" s="38"/>
+      <c r="BB5" s="38"/>
+      <c r="BC5" s="38"/>
+      <c r="BD5" s="38"/>
+      <c r="BE5" s="38"/>
+      <c r="BF5" s="37"/>
+      <c r="BG5" s="38"/>
+      <c r="BH5" s="38"/>
+      <c r="BI5" s="38"/>
+      <c r="BJ5" s="38"/>
+      <c r="BK5" s="38"/>
+      <c r="BL5" s="38"/>
+      <c r="BM5" s="38"/>
+      <c r="BN5" s="37"/>
+      <c r="BO5" s="38"/>
     </row>
     <row r="6" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="54" t="s">
         <v>60</v>
       </c>
       <c r="D6" s="3"/>
@@ -2639,7 +2873,7 @@
     </row>
     <row r="7" spans="1:67" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
-      <c r="C7" s="41"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -2706,14 +2940,14 @@
       <c r="BO7" s="3"/>
     </row>
     <row r="8" spans="1:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="46">
-        <v>1</v>
-      </c>
-      <c r="B8" s="61" t="s">
+      <c r="A8" s="45">
+        <v>1</v>
+      </c>
+      <c r="B8" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="44"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="43"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -2721,15 +2955,15 @@
       <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:67" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="47">
+      <c r="A9" s="46">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="57" t="s">
         <v>123</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="29" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E9" s="14">
         <v>1</v>
@@ -2748,15 +2982,15 @@
       </c>
     </row>
     <row r="10" spans="1:67" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47">
+      <c r="A10" s="46">
         <v>1.2</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="57" t="s">
         <v>67</v>
       </c>
       <c r="C10" s="28"/>
       <c r="D10" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E10" s="14">
         <v>1</v>
@@ -2775,15 +3009,15 @@
       </c>
     </row>
     <row r="11" spans="1:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="47">
+      <c r="A11" s="46">
         <v>1.3</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="57" t="s">
         <v>68</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E11" s="14">
         <v>1</v>
@@ -2802,10 +3036,10 @@
       </c>
     </row>
     <row r="12" spans="1:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="47">
+      <c r="A12" s="46">
         <v>1.4</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="57" t="s">
         <v>69</v>
       </c>
       <c r="C12" s="28"/>
@@ -2829,15 +3063,15 @@
       </c>
     </row>
     <row r="13" spans="1:67" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="47">
+      <c r="A13" s="46">
         <v>1.5</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="57" t="s">
         <v>70</v>
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="29" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E13" s="14">
         <v>1</v>
@@ -2856,14 +3090,14 @@
       </c>
     </row>
     <row r="14" spans="1:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46">
+      <c r="A14" s="45">
         <v>2</v>
       </c>
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="59" t="s">
         <v>102</v>
       </c>
       <c r="C14" s="28"/>
-      <c r="D14" s="44"/>
+      <c r="D14" s="43"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
@@ -2871,15 +3105,15 @@
       <c r="I14" s="15"/>
     </row>
     <row r="15" spans="1:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="47">
+      <c r="A15" s="46">
         <v>2.1</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="57" t="s">
         <v>113</v>
       </c>
       <c r="C15" s="28"/>
       <c r="D15" s="29" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E15" s="14">
         <v>5</v>
@@ -2898,10 +3132,10 @@
       </c>
     </row>
     <row r="16" spans="1:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="47">
+      <c r="A16" s="46">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="57" t="s">
         <v>114</v>
       </c>
       <c r="C16" s="28"/>
@@ -2925,15 +3159,15 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47">
+      <c r="A17" s="46">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="57" t="s">
         <v>74</v>
       </c>
       <c r="C17" s="28"/>
       <c r="D17" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E17" s="14">
         <v>5</v>
@@ -2952,15 +3186,15 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47">
+      <c r="A18" s="46">
         <v>2.4</v>
       </c>
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="57" t="s">
         <v>75</v>
       </c>
       <c r="C18" s="28"/>
       <c r="D18" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E18" s="14">
         <v>5</v>
@@ -2979,15 +3213,15 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="47">
+      <c r="A19" s="46">
         <v>2.5</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="57" t="s">
         <v>76</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="29" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E19" s="14">
         <v>5</v>
@@ -3006,10 +3240,10 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="47">
+      <c r="A20" s="46">
         <v>2.6</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="57" t="s">
         <v>77</v>
       </c>
       <c r="C20" s="28"/>
@@ -3033,10 +3267,10 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="47">
+      <c r="A21" s="46">
         <v>2.7</v>
       </c>
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="57" t="s">
         <v>78</v>
       </c>
       <c r="C21" s="28"/>
@@ -3060,13 +3294,13 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="46">
+      <c r="A22" s="45">
         <v>3</v>
       </c>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="D22" s="42"/>
+      <c r="D22" s="41"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -3074,15 +3308,15 @@
       <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="47">
+      <c r="A23" s="46">
         <v>3.1</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="57" t="s">
         <v>79</v>
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="29" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E23" s="14">
         <v>10</v>
@@ -3101,15 +3335,15 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="47">
+      <c r="A24" s="46">
         <v>3.2</v>
       </c>
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="57" t="s">
         <v>115</v>
       </c>
       <c r="C24" s="28"/>
       <c r="D24" s="29" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E24" s="14">
         <v>10</v>
@@ -3128,15 +3362,15 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47">
+      <c r="A25" s="46">
         <v>3.3</v>
       </c>
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="57" t="s">
         <v>82</v>
       </c>
       <c r="C25" s="28"/>
       <c r="D25" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E25" s="14">
         <v>10</v>
@@ -3147,19 +3381,23 @@
       <c r="G25" s="14">
         <v>14</v>
       </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="15"/>
+      <c r="H25" s="14">
+        <v>3</v>
+      </c>
+      <c r="I25" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="47">
+      <c r="A26" s="46">
         <v>3.4</v>
       </c>
-      <c r="B26" s="58" t="s">
+      <c r="B26" s="57" t="s">
         <v>83</v>
       </c>
       <c r="C26" s="28"/>
       <c r="D26" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E26" s="14">
         <v>10</v>
@@ -3170,14 +3408,18 @@
       <c r="G26" s="14">
         <v>14</v>
       </c>
-      <c r="H26" s="14"/>
-      <c r="I26" s="15"/>
+      <c r="H26" s="14">
+        <v>3</v>
+      </c>
+      <c r="I26" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="47">
+      <c r="A27" s="46">
         <v>3.5</v>
       </c>
-      <c r="B27" s="58" t="s">
+      <c r="B27" s="57" t="s">
         <v>84</v>
       </c>
       <c r="C27" s="28"/>
@@ -3201,10 +3443,10 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="47">
+      <c r="A28" s="46">
         <v>3.6</v>
       </c>
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="57" t="s">
         <v>116</v>
       </c>
       <c r="C28" s="28"/>
@@ -3228,15 +3470,15 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="47">
+      <c r="A29" s="46">
         <v>3.7</v>
       </c>
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="57" t="s">
         <v>117</v>
       </c>
       <c r="C29" s="28"/>
       <c r="D29" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E29" s="14">
         <v>10</v>
@@ -3247,19 +3489,23 @@
       <c r="G29" s="14">
         <v>14</v>
       </c>
-      <c r="H29" s="14"/>
-      <c r="I29" s="15"/>
+      <c r="H29" s="14">
+        <v>5</v>
+      </c>
+      <c r="I29" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="47">
+      <c r="A30" s="46">
         <v>3.8</v>
       </c>
-      <c r="B30" s="58" t="s">
+      <c r="B30" s="57" t="s">
         <v>87</v>
       </c>
       <c r="C30" s="28"/>
       <c r="D30" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E30" s="14">
         <v>10</v>
@@ -3270,14 +3516,18 @@
       <c r="G30" s="14">
         <v>14</v>
       </c>
-      <c r="H30" s="14"/>
-      <c r="I30" s="15"/>
+      <c r="H30" s="14">
+        <v>4</v>
+      </c>
+      <c r="I30" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="47">
+      <c r="A31" s="46">
         <v>3.9</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="57" t="s">
         <v>88</v>
       </c>
       <c r="C31" s="28"/>
@@ -3301,15 +3551,15 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="47">
+      <c r="A32" s="46">
         <v>3.1</v>
       </c>
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="57" t="s">
         <v>89</v>
       </c>
       <c r="C32" s="28"/>
       <c r="D32" s="29" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E32" s="14">
         <v>10</v>
@@ -3328,10 +3578,10 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="47">
+      <c r="A33" s="46">
         <v>3.11</v>
       </c>
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="57" t="s">
         <v>90</v>
       </c>
       <c r="C33" s="28"/>
@@ -3355,13 +3605,13 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="46">
+      <c r="A34" s="45">
         <v>4</v>
       </c>
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="42"/>
+      <c r="D34" s="41"/>
       <c r="E34" s="14"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
@@ -3369,29 +3619,37 @@
       <c r="I34" s="15"/>
     </row>
     <row r="35" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="47">
+      <c r="A35" s="46">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B35" s="58" t="s">
+      <c r="B35" s="57" t="s">
         <v>91</v>
       </c>
       <c r="C35" s="28"/>
       <c r="D35" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E35" s="14">
         <v>19</v>
       </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="15"/>
+      <c r="F35" s="14">
+        <v>5</v>
+      </c>
+      <c r="G35" s="14">
+        <v>28</v>
+      </c>
+      <c r="H35" s="14">
+        <v>2</v>
+      </c>
+      <c r="I35" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="47">
+      <c r="A36" s="46">
         <v>4.2</v>
       </c>
-      <c r="B36" s="58" t="s">
+      <c r="B36" s="57" t="s">
         <v>92</v>
       </c>
       <c r="C36" s="28"/>
@@ -3415,10 +3673,10 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="46">
+      <c r="A37" s="45">
         <v>5</v>
       </c>
-      <c r="B37" s="60" t="s">
+      <c r="B37" s="59" t="s">
         <v>105</v>
       </c>
       <c r="C37" s="28"/>
@@ -3430,15 +3688,15 @@
       <c r="I37" s="15"/>
     </row>
     <row r="38" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="47">
+      <c r="A38" s="46">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B38" s="58" t="s">
+      <c r="B38" s="57" t="s">
         <v>93</v>
       </c>
       <c r="C38" s="28"/>
       <c r="D38" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E38" s="14">
         <v>19</v>
@@ -3446,15 +3704,21 @@
       <c r="F38" s="14">
         <v>5</v>
       </c>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="15"/>
+      <c r="G38" s="14">
+        <v>28</v>
+      </c>
+      <c r="H38" s="14">
+        <v>3</v>
+      </c>
+      <c r="I38" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="47">
+      <c r="A39" s="46">
         <v>5.2</v>
       </c>
-      <c r="B39" s="58" t="s">
+      <c r="B39" s="57" t="s">
         <v>94</v>
       </c>
       <c r="C39" s="28"/>
@@ -3470,17 +3734,21 @@
       <c r="G39" s="14">
         <v>20</v>
       </c>
-      <c r="H39" s="14"/>
-      <c r="I39" s="15"/>
+      <c r="H39" s="14">
+        <v>2</v>
+      </c>
+      <c r="I39" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="46">
+      <c r="A40" s="45">
         <v>6</v>
       </c>
-      <c r="B40" s="60" t="s">
+      <c r="B40" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="D40" s="42"/>
+      <c r="D40" s="41"/>
       <c r="E40" s="14"/>
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
@@ -3488,15 +3756,15 @@
       <c r="I40" s="15"/>
     </row>
     <row r="41" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="47">
+      <c r="A41" s="46">
         <v>6.1</v>
       </c>
-      <c r="B41" s="58" t="s">
+      <c r="B41" s="57" t="s">
         <v>87</v>
       </c>
       <c r="C41" s="28"/>
       <c r="D41" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E41" s="14">
         <v>19</v>
@@ -3504,20 +3772,26 @@
       <c r="F41" s="14">
         <v>5</v>
       </c>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="15"/>
+      <c r="G41" s="14">
+        <v>28</v>
+      </c>
+      <c r="H41" s="14">
+        <v>3</v>
+      </c>
+      <c r="I41" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="47">
+      <c r="A42" s="46">
         <v>6.2</v>
       </c>
-      <c r="B42" s="58" t="s">
+      <c r="B42" s="57" t="s">
         <v>88</v>
       </c>
       <c r="C42" s="28"/>
       <c r="D42" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E42" s="14">
         <v>19</v>
@@ -3525,20 +3799,26 @@
       <c r="F42" s="14">
         <v>5</v>
       </c>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="15"/>
+      <c r="G42" s="14">
+        <v>28</v>
+      </c>
+      <c r="H42" s="14">
+        <v>3</v>
+      </c>
+      <c r="I42" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="47">
+      <c r="A43" s="46">
         <v>6.3</v>
       </c>
-      <c r="B43" s="58" t="s">
+      <c r="B43" s="57" t="s">
         <v>89</v>
       </c>
       <c r="C43" s="28"/>
       <c r="D43" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E43" s="14">
         <v>19</v>
@@ -3546,20 +3826,26 @@
       <c r="F43" s="14">
         <v>5</v>
       </c>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="15"/>
+      <c r="G43" s="14">
+        <v>28</v>
+      </c>
+      <c r="H43" s="14">
+        <v>2</v>
+      </c>
+      <c r="I43" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="47">
+      <c r="A44" s="46">
         <v>6.4</v>
       </c>
-      <c r="B44" s="58" t="s">
+      <c r="B44" s="57" t="s">
         <v>95</v>
       </c>
       <c r="C44" s="28"/>
       <c r="D44" s="29" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E44" s="14">
         <v>19</v>
@@ -3570,19 +3856,23 @@
       <c r="G44" s="14">
         <v>22</v>
       </c>
-      <c r="H44" s="14"/>
-      <c r="I44" s="15"/>
+      <c r="H44" s="14">
+        <v>4</v>
+      </c>
+      <c r="I44" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="47">
+      <c r="A45" s="46">
         <v>6.5</v>
       </c>
-      <c r="B45" s="58" t="s">
+      <c r="B45" s="57" t="s">
         <v>96</v>
       </c>
       <c r="C45" s="28"/>
       <c r="D45" s="29" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E45" s="14">
         <v>19</v>
@@ -3597,19 +3887,19 @@
         <v>1</v>
       </c>
       <c r="I45" s="15">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="47">
+      <c r="A46" s="46">
         <v>6.6</v>
       </c>
-      <c r="B46" s="58" t="s">
+      <c r="B46" s="57" t="s">
         <v>97</v>
       </c>
       <c r="C46" s="28"/>
       <c r="D46" s="29" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E46" s="14">
         <v>19</v>
@@ -3617,20 +3907,26 @@
       <c r="F46" s="14">
         <v>5</v>
       </c>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="15"/>
+      <c r="G46" s="14">
+        <v>27</v>
+      </c>
+      <c r="H46" s="14">
+        <v>1</v>
+      </c>
+      <c r="I46" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="47">
+      <c r="A47" s="46">
         <v>6.7</v>
       </c>
-      <c r="B47" s="58" t="s">
+      <c r="B47" s="57" t="s">
         <v>98</v>
       </c>
       <c r="C47" s="28"/>
       <c r="D47" s="29" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="E47" s="14">
         <v>19</v>
@@ -3638,18 +3934,24 @@
       <c r="F47" s="14">
         <v>5</v>
       </c>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="15"/>
+      <c r="G47" s="14">
+        <v>28</v>
+      </c>
+      <c r="H47" s="14">
+        <v>2</v>
+      </c>
+      <c r="I47" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="46">
+      <c r="A48" s="45">
         <v>7</v>
       </c>
-      <c r="B48" s="60" t="s">
+      <c r="B48" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="D48" s="42"/>
+      <c r="D48" s="41"/>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
       <c r="G48" s="14"/>
@@ -3657,10 +3959,10 @@
       <c r="I48" s="15"/>
     </row>
     <row r="49" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="47">
+      <c r="A49" s="46">
         <v>7.1</v>
       </c>
-      <c r="B49" s="58" t="s">
+      <c r="B49" s="57" t="s">
         <v>121</v>
       </c>
       <c r="C49" s="28"/>
@@ -3684,15 +3986,15 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="47">
+      <c r="A50" s="46">
         <v>7.2</v>
       </c>
-      <c r="B50" s="58" t="s">
+      <c r="B50" s="57" t="s">
         <v>99</v>
       </c>
       <c r="C50" s="28"/>
       <c r="D50" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E50" s="14">
         <v>19</v>
@@ -3700,20 +4002,26 @@
       <c r="F50" s="14">
         <v>10</v>
       </c>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="15"/>
+      <c r="G50" s="14">
+        <v>28</v>
+      </c>
+      <c r="H50" s="14">
+        <v>2</v>
+      </c>
+      <c r="I50" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="47">
+      <c r="A51" s="46">
         <v>7.3</v>
       </c>
-      <c r="B51" s="58" t="s">
+      <c r="B51" s="57" t="s">
         <v>100</v>
       </c>
       <c r="C51" s="28"/>
       <c r="D51" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E51" s="14">
         <v>19</v>
@@ -3721,20 +4029,26 @@
       <c r="F51" s="14">
         <v>10</v>
       </c>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="15"/>
+      <c r="G51" s="14">
+        <v>28</v>
+      </c>
+      <c r="H51" s="14">
+        <v>4</v>
+      </c>
+      <c r="I51" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="47">
+      <c r="A52" s="46">
         <v>7.4</v>
       </c>
-      <c r="B52" s="58" t="s">
+      <c r="B52" s="57" t="s">
         <v>101</v>
       </c>
       <c r="C52" s="28"/>
       <c r="D52" s="29" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E52" s="14">
         <v>19</v>
@@ -3742,18 +4056,24 @@
       <c r="F52" s="14">
         <v>10</v>
       </c>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="15"/>
+      <c r="G52" s="14">
+        <v>25</v>
+      </c>
+      <c r="H52" s="14">
+        <v>1</v>
+      </c>
+      <c r="I52" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="48"/>
+      <c r="A53" s="47"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="48"/>
+      <c r="A54" s="47"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="48"/>
+      <c r="A55" s="47"/>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
@@ -3851,14 +4171,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A2:D24"/>
   <sheetViews>
     <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3869,101 +4189,101 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="49" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="65" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="64">
+    <row r="3" spans="1:4" s="64" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="63">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="66" t="s">
+      <c r="B3" s="63"/>
+      <c r="C3" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="D3" s="64"/>
+      <c r="D3" s="63"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>2.1</v>
       </c>
       <c r="B4" s="17"/>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="57" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="57" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="59">
+      <c r="A6" s="58">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="57" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="57" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="59">
+      <c r="A8" s="58">
         <v>3.2</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="57" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="57" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="59">
+      <c r="A10" s="58">
         <v>3.6</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="57" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="59">
+      <c r="A11" s="58">
         <v>3.7</v>
       </c>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="57" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="59">
+      <c r="A12" s="58">
         <v>7.1</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="57" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
-      <c r="C21" s="49"/>
+      <c r="C21" s="48"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
-      <c r="B24" s="51"/>
+      <c r="B24" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>